<commit_message>
fix mapa so parecer
</commit_message>
<xml_diff>
--- a/statics/MAPA_FINAL_2023_SO_PARECER.xlsx
+++ b/statics/MAPA_FINAL_2023_SO_PARECER.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f28ae49758e922e1/Desktop/devbook/editabletable/statics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{4345199E-B276-46ED-BCB8-7FB98B789D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{664CA0CF-D817-49AA-8465-A139D4A040B9}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{4345199E-B276-46ED-BCB8-7FB98B789D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9CA63B3-EAB7-4131-948C-2DD07E66407B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCAD9878-E9D0-420E-8A55-493979D05A8F}"/>
   </bookViews>
@@ -39,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Turma:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Educação para a esperança e transformação!</t>
   </si>
@@ -229,14 +226,8 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -250,23 +241,29 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -298,6 +295,65 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>130476</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1449883</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1" descr="Logotipo, nome da empresa&#10;&#10;Descrição gerada automaticamente">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D73789E8-CB62-4E68-B6C6-3CAD4096209E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="130476" y="0"/>
+          <a:ext cx="1319407" cy="1287780"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -604,222 +660,250 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5:B5"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="2" width="50.109375" customWidth="1"/>
-    <col min="3" max="3" width="52.21875" customWidth="1"/>
+    <col min="3" max="3" width="50.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="47.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:3" ht="86.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3"/>
+      <c r="B1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="11"/>
-    </row>
-    <row r="2" spans="1:3" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="10"/>
-    </row>
-    <row r="3" spans="1:3" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="15"/>
-      <c r="B3" s="12" t="s">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" ht="43.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="12"/>
-    </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="14"/>
+      <c r="C4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="5" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="7"/>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="7"/>
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="7"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="7"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="9"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="7"/>
       <c r="C22" s="2"/>
     </row>
     <row r="23" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="7"/>
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
-      <c r="B26" s="9"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
       <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="5"/>
       <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="9"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="9"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="7"/>
       <c r="C30" s="2"/>
     </row>
     <row r="31" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6"/>
-      <c r="B31" s="7"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="8"/>
-      <c r="B32" s="9"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="5"/>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
-      <c r="B34" s="9"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
       <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="6"/>
-      <c r="B35" s="7"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="8"/>
-      <c r="B36" s="9"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="7"/>
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6"/>
-      <c r="B37" s="7"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="5"/>
       <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="7"/>
       <c r="C38" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -829,36 +913,6 @@
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:C38">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
@@ -867,5 +921,6 @@
   </conditionalFormatting>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.15748031496062992" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="80" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajustes em modelo do parecer final
</commit_message>
<xml_diff>
--- a/statics/MAPA_FINAL_2023_SO_PARECER.xlsx
+++ b/statics/MAPA_FINAL_2023_SO_PARECER.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f28ae49758e922e1/Desktop/devbook/editabletable/statics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jw_wi\OneDrive\Desktop\devbook\editabletable\statics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{4345199E-B276-46ED-BCB8-7FB98B789D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9CA63B3-EAB7-4131-948C-2DD07E66407B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B262038-237C-429B-8812-3F758084CC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCAD9878-E9D0-420E-8A55-493979D05A8F}"/>
   </bookViews>
@@ -95,13 +95,6 @@
       <family val="4"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="22"/>
       <color theme="1"/>
@@ -122,6 +115,13 @@
       <color theme="1"/>
       <name val="Cavolini"/>
       <family val="4"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -220,50 +220,50 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -350,10 +350,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -660,7 +656,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:B4"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,239 +667,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="86.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="3"/>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:3" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="7"/>
     </row>
     <row r="4" spans="1:3" ht="43.2" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="9"/>
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="1"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="2"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
     </row>
     <row r="7" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="1"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="2"/>
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="1"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="2"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
     </row>
     <row r="11" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="2"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
     </row>
     <row r="13" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="2"/>
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
     </row>
     <row r="15" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="6"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="15"/>
     </row>
     <row r="17" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="1"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="2"/>
+      <c r="A18" s="13"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
     </row>
     <row r="19" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="13"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="15"/>
     </row>
     <row r="21" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="1"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
     </row>
     <row r="22" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="6"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="2"/>
+      <c r="A22" s="13"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
     </row>
     <row r="23" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="1"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="2"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="1"/>
+      <c r="A25" s="10"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="12"/>
     </row>
     <row r="26" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="2"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="15"/>
     </row>
     <row r="27" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="1"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
     </row>
     <row r="28" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="2"/>
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
     </row>
     <row r="29" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="1"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="12"/>
     </row>
     <row r="30" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="6"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="2"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
     </row>
     <row r="31" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="1"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="12"/>
     </row>
     <row r="32" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="6"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="2"/>
+      <c r="A32" s="13"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="15"/>
     </row>
     <row r="33" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="4"/>
-      <c r="B33" s="5"/>
-      <c r="C33" s="1"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="12"/>
     </row>
     <row r="34" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="2"/>
+      <c r="A34" s="13"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="15"/>
     </row>
     <row r="35" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="4"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="1"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="12"/>
     </row>
     <row r="36" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="2"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="1"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:3" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="6"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="2"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="A37:B37"/>
@@ -913,6 +879,36 @@
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:C38">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">

</xml_diff>